<commit_message>
Okay, I have the first problems done.
More to follow.
</commit_message>
<xml_diff>
--- a/ExcelEsport/Day1.xlsx
+++ b/ExcelEsport/Day1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/ExcelEsport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F10518B7-3F66-4E79-ACC9-14DFEA7864DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{F10518B7-3F66-4E79-ACC9-14DFEA7864DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66B7FDD3-5113-4731-865B-A2568B1F6CAB}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>FROM:</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>Text Drill</t>
+  </si>
+  <si>
+    <t>How many Gmail addresses?</t>
+  </si>
+  <si>
+    <t>How many email addresses?</t>
+  </si>
+  <si>
+    <t>Marleen Siemon, Adi Bedivere Hoekstra, Clemence Krüger, Marzanna Aviram D'Antonio, Nkiru Cantu, Petros Holmwood, Edmundas Kuno Fannon, Dzvezda Juhån Nikolic, Chanda Björk, Hjørdis Rivers, Herleifr Milan Dresdner, Kerenza Inken Ko, Maria Teresa Erna Sundberg, Clemence Damianus De Bruijn, Quinctilius Shanthi Dirix, Ridwana Lisa Holmgren, Julienne Roth, Hazel Alger, Danr North, Olegarius Fierro</t>
   </si>
 </sst>
 </file>
@@ -379,7 +388,7 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -392,7 +401,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="17"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
@@ -701,10 +709,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9503465</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>496625</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>15505</xdr:rowOff>
+      <xdr:rowOff>19315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -729,6 +737,50 @@
         <a:xfrm>
           <a:off x="609600" y="1028700"/>
           <a:ext cx="9497750" cy="1895740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>250934</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76426</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1CA35C3-696A-F2C5-89F6-4ADF6E6EDFF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="4972050"/>
+          <a:ext cx="9878804" cy="1619476"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -868,7 +920,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1160,15 +1212,15 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1199,9 +1251,32 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24">
+        <f>LEN(B21)-LEN(SUBSTITUTE(B21,"@",""))</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25">
+        <f>(LEN(B21)-LEN(SUBSTITUTE(B21,"gmail","")))/LEN("gmail")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1390,19 +1465,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -1410,11 +1481,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -1422,19 +1492,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -1442,11 +1508,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -1454,19 +1519,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -1474,11 +1535,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -1486,13 +1546,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finally did all the drills
</commit_message>
<xml_diff>
--- a/ExcelEsport/Day1.xlsx
+++ b/ExcelEsport/Day1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/ExcelEsport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{F10518B7-3F66-4E79-ACC9-14DFEA7864DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66B7FDD3-5113-4731-865B-A2568B1F6CAB}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{F10518B7-3F66-4E79-ACC9-14DFEA7864DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54F02DD5-AA0D-46CF-9435-DBD065260D2F}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -18,11 +18,13 @@
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="emails">Report!$B$21</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
+    <definedName name="names">Report!$B$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="9" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>FROM:</t>
   </si>
@@ -157,6 +159,12 @@
   </si>
   <si>
     <t>Marleen Siemon, Adi Bedivere Hoekstra, Clemence Krüger, Marzanna Aviram D'Antonio, Nkiru Cantu, Petros Holmwood, Edmundas Kuno Fannon, Dzvezda Juhån Nikolic, Chanda Björk, Hjørdis Rivers, Herleifr Milan Dresdner, Kerenza Inken Ko, Maria Teresa Erna Sundberg, Clemence Damianus De Bruijn, Quinctilius Shanthi Dirix, Ridwana Lisa Holmgren, Julienne Roth, Hazel Alger, Danr North, Olegarius Fierro</t>
+  </si>
+  <si>
+    <t>People more than two names</t>
+  </si>
+  <si>
+    <t>People</t>
   </si>
 </sst>
 </file>
@@ -710,7 +718,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>496625</xdr:colOff>
+      <xdr:colOff>54665</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>19315</xdr:rowOff>
     </xdr:to>
@@ -748,15 +756,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>97155</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>250934</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>76426</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>416669</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>19276</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -779,8 +787,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="4972050"/>
-          <a:ext cx="9878804" cy="1619476"/>
+          <a:off x="617220" y="5583555"/>
+          <a:ext cx="9861659" cy="1625191"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -839,6 +847,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -920,7 +932,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1212,15 +1224,15 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="18" max="18" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1247,16 +1259,16 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>09-Jan-2024</v>
+        <v>10-Jan-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>29</v>
       </c>
@@ -1265,7 +1277,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>28</v>
       </c>
@@ -1273,10 +1285,188 @@
         <f>(LEN(B21)-LEN(SUBSTITUTE(B21,"gmail","")))/LEN("gmail")</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="R25" t="str" cm="1">
+        <f t="array" ref="R25:S41">_xlfn.TEXTSPLIT(emails,"@",";")</f>
+        <v>eve.kupha131</v>
+      </c>
+      <c r="S25" t="str">
+        <v>gmail.com</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R26" t="str">
+        <v xml:space="preserve"> damion.senger64</v>
+      </c>
+      <c r="S26" t="str">
+        <v>yahoo.com</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" t="str" cm="1">
+        <f t="array" ref="B27:C29">_xlfn.LET(_xlpm.split,_xlfn.TEXTSPLIT(emails,"@","; "),
+     _xlpm.domains,_xlfn.UNIQUE(_xlfn.TAKE(_xlpm.split,,-1)),
+     _xlpm.count,(LEN(emails)-LEN(SUBSTITUTE(emails,_xlpm.domains,"")))/LEN(_xlpm.domains),
+     _xlfn._xlws.SORT(_xlfn.HSTACK(_xlpm.domains,_xlpm.count),2,-1))</f>
+        <v>gmail.com</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="R27" t="str">
+        <v xml:space="preserve"> danial.botsford</v>
+      </c>
+      <c r="S27" t="str">
+        <v>gmail.com</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" t="str">
+        <v>hotmail.com</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="R28" t="str">
+        <v xml:space="preserve"> harley55</v>
+      </c>
+      <c r="S28" t="str">
+        <v>gmail.com</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" t="str">
+        <v>yahoo.com</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="R29" t="str">
+        <v xml:space="preserve"> marco moen81</v>
+      </c>
+      <c r="S29" t="str">
+        <v>yahoo.com</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R30" t="str">
+        <v xml:space="preserve"> demarco.gulgowski</v>
+      </c>
+      <c r="S30" t="str">
+        <v>hotmail.com</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R31" t="str">
+        <v xml:space="preserve"> cooper.harber</v>
+      </c>
+      <c r="S31" t="str">
+        <v>gmail.com</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R32" t="str">
+        <v xml:space="preserve"> veda.reynolds72</v>
+      </c>
+      <c r="S32" t="str">
+        <v>hotmail.com</v>
+      </c>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R33" t="str">
+        <v xml:space="preserve"> helen68</v>
+      </c>
+      <c r="S33" t="str">
+        <v>gmail.com</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R34" t="str">
+        <v xml:space="preserve"> elyssa10</v>
+      </c>
+      <c r="S34" t="str">
+        <v>hotmail.com</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R35" t="str">
+        <v xml:space="preserve"> keara_predovic</v>
+      </c>
+      <c r="S35" t="str">
+        <v>gmail.com</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R36" t="str">
+        <v xml:space="preserve"> kitty_treute163</v>
+      </c>
+      <c r="S36" t="str">
+        <v>hotmail.com</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R37" t="str">
+        <v xml:space="preserve"> emmanuel.wuckert32</v>
+      </c>
+      <c r="S37" t="str">
+        <v>hotmail.com</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R38" t="str">
+        <v xml:space="preserve"> kade_yundt</v>
+      </c>
+      <c r="S38" t="str">
+        <v>gmail.com</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R39" t="str">
+        <v xml:space="preserve"> mario_prosacc096</v>
+      </c>
+      <c r="S39" t="str">
+        <v>yahoo.com</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R40" t="str">
+        <v xml:space="preserve"> mazie_cruickshank70</v>
+      </c>
+      <c r="S40" t="str">
+        <v>yahoo.com</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R41" t="str">
+        <v xml:space="preserve"> winifred.koss35</v>
+      </c>
+      <c r="S41" t="str">
+        <v>hotmail.com</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46">
+        <f>LEN(names)-LEN(SUBSTITUTE(names,",",""))+1</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47">
+        <f>_xlfn.LET(_xlpm.split,_xlfn.TEXTSPLIT(names," ",", "),
+     _xlpm.third,_xlfn.CHOOSECOLS(_xlpm.split,3),
+     _xlpm.nonErr,_xlfn.TOCOL(_xlpm.third,2),
+     ROWS(_xlpm.nonErr))</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1328,7 +1518,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>09-Jan-2024</v>
+        <v>10-Jan-2024</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1638,7 +1828,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>09-Jan-2024</v>
+        <v>10-Jan-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>